<commit_message>
add excel and sentences
</commit_message>
<xml_diff>
--- a/DEMO.xlsx
+++ b/DEMO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor-PC\OneDrive\FullStack\Project\crmsms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{231AA9D5-7D00-4249-BD04-F96196354F52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A88FB0E9-4E72-45A8-8CC1-0A3ED9560CFB}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{231AA9D5-7D00-4249-BD04-F96196354F52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E92B4561-CF76-4C88-9CFD-687D4F380334}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
   <si>
     <t>Phone Number</t>
   </si>
@@ -37,13 +37,13 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>לידור</t>
+    <t>0526761204</t>
   </si>
   <si>
-    <t>מליח</t>
+    <t>ישראלי</t>
   </si>
   <si>
-    <t>0526761204</t>
+    <t>ישראל</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -385,83 +385,173 @@
     </row>
     <row r="2" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>6</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="8">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
add excel gui import
</commit_message>
<xml_diff>
--- a/DEMO.xlsx
+++ b/DEMO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor-PC\OneDrive\FullStack\Project\crmsms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor-PC\Documents\Git\crmsms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{231AA9D5-7D00-4249-BD04-F96196354F52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E92B4561-CF76-4C88-9CFD-687D4F380334}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7052CD-982F-49B8-A751-390C46C3B790}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t>Phone Number</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Number Of Guests</t>
-  </si>
-  <si>
-    <t>Number Of Guests Accept</t>
   </si>
   <si>
     <t>First Name</t>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>ישראל</t>
+  </si>
+  <si>
+    <t>משה</t>
   </si>
 </sst>
 </file>
@@ -343,7 +343,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -361,7 +361,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -369,9 +369,7 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -385,171 +383,141 @@
     </row>
     <row r="2" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D5" s="8">
         <v>4</v>
       </c>
-      <c r="E5" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="8">
         <v>5</v>
       </c>
-      <c r="E6" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D7" s="8">
         <v>6</v>
       </c>
-      <c r="E7" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="8">
         <v>7</v>
       </c>
-      <c r="E8" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="9" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D9" s="8">
         <v>8</v>
       </c>
-      <c r="E9" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="10" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="8">
         <v>9</v>
       </c>
-      <c r="E10" s="8">
-        <v>2</v>
-      </c>
     </row>
     <row r="11" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="D11" s="8">
-        <v>10</v>
-      </c>
-      <c r="E11" s="8">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dashboard UI and delete some components
</commit_message>
<xml_diff>
--- a/DEMO.xlsx
+++ b/DEMO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor-PC\Documents\Git\crmsms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A29835-8C60-4480-B3F6-CDC7D59B396B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF6E12-8FB1-4B69-8265-5F0FB2A2D9E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>Phone Number</t>
   </si>
@@ -44,6 +44,33 @@
   </si>
   <si>
     <t>ישראל</t>
+  </si>
+  <si>
+    <t>0526761205</t>
+  </si>
+  <si>
+    <t>0526761206</t>
+  </si>
+  <si>
+    <t>0526761207</t>
+  </si>
+  <si>
+    <t>0526761208</t>
+  </si>
+  <si>
+    <t>0526761209</t>
+  </si>
+  <si>
+    <t>0526761210</t>
+  </si>
+  <si>
+    <t>0526761211</t>
+  </si>
+  <si>
+    <t>0526761212</t>
+  </si>
+  <si>
+    <t>0526761213</t>
   </si>
 </sst>
 </file>
@@ -95,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -129,9 +156,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
@@ -361,7 +385,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -414,128 +438,128 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="14">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+    </row>
+    <row r="6" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="D7" s="14">
         <v>6</v>
       </c>
-      <c r="C4" s="14" t="s">
+    </row>
+    <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="D8" s="14">
         <v>7</v>
       </c>
-      <c r="C5" s="14" t="s">
+    </row>
+    <row r="9" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="D9" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D10" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="15">
+      <c r="D11" s="14">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add group import in excel
</commit_message>
<xml_diff>
--- a/DEMO.xlsx
+++ b/DEMO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor-PC\Documents\Git\crmsms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AAFBAC-28F1-4372-A396-DCBF6829EF38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306C9909-F7D5-4B1D-8F18-FE7370C4BD83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Phone Number</t>
   </si>
@@ -96,6 +96,9 @@
   <si>
     <t>חנה</t>
   </si>
+  <si>
+    <t>Event Group</t>
+  </si>
 </sst>
 </file>
 
@@ -112,17 +115,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -409,7 +415,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -435,7 +441,9 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>

</xml_diff>